<commit_message>
GameViewController: Add popover for iPad when sharing, because it crashes if it's missing. Organize HowToPlay, Purchase, and Settings into folders. ParentPage: made padding static. HowToPlayTableView: update instructions. PurchasePage and PurchaseTapButton: add these files SettingsPage: update padding to use static version. SettingsTapButton: refactor. PauseResetEngine: remove comingSoonLabel. Implement PurchasePage. Remove silence at beginning of buttontap5.mp3. Extension+UIImage: add purchaseButtonGradientTexture GameScene: delete touchesMoved. DecisionButtonSprite: remove the mask and crop node; these were proof of concepts when creating PurchaseTapButton.
</commit_message>
<xml_diff>
--- a/JSON/Levels13MoveList.xlsx
+++ b/JSON/Levels13MoveList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10794193-A280-F14B-8EAF-D1EF67E1F295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E0E67E-6930-B446-AFB3-EDE47BDB6094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18099" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18281" uniqueCount="156">
   <si>
     <t>health</t>
   </si>
@@ -364,12 +364,168 @@
   <si>
     <t>Move Count Check</t>
   </si>
+  <si>
+    <t>R,L,D,R,R,U,R,U,U,R,R,D,R,R,U,U,U,L,U,L,D,R,U,R,D,R,R,U,U,D</t>
+  </si>
+  <si>
+    <t>R,R,L,L,D,D,R,R</t>
+  </si>
+  <si>
+    <t>R,U,D,D,L,L,U,U</t>
+  </si>
+  <si>
+    <t>D,D,U,R,R,U,D,D</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,D,R,D,L,U</t>
+    </r>
+  </si>
+  <si>
+    <t>U,U,R,R,D,D,L,R</t>
+  </si>
+  <si>
+    <t>R,R,D,D,L,L,U,R</t>
+  </si>
+  <si>
+    <t>R,R,D,D,L,L,R,R</t>
+  </si>
+  <si>
+    <t>D,U,R,R,D,D</t>
+  </si>
+  <si>
+    <t>D,R,R,U,D,D</t>
+  </si>
+  <si>
+    <t>R,R,L,D,D,L,R,R</t>
+  </si>
+  <si>
+    <t>U,D,L,R,R,L,D,R</t>
+  </si>
+  <si>
+    <t>R,L,D,D,R,R,U,D</t>
+  </si>
+  <si>
+    <t>R,R,D,D,L,L,U,D,R,R</t>
+  </si>
+  <si>
+    <t>R,D,D,U,U,R</t>
+  </si>
+  <si>
+    <t>D,D,R,R,U,U,L,L,D</t>
+  </si>
+  <si>
+    <t>R,D,L,L</t>
+  </si>
+  <si>
+    <t>D,D,U,U,R,D</t>
+  </si>
+  <si>
+    <t>D,D,D,D</t>
+  </si>
+  <si>
+    <t>R,R,D,U,D,D,U,U,R</t>
+  </si>
+  <si>
+    <t>R,D,U,D,R,D,U,U</t>
+  </si>
+  <si>
+    <t>R,U,D,U,D,D,U,D</t>
+  </si>
+  <si>
+    <t>R,D,U,D,D,R</t>
+  </si>
+  <si>
+    <t>R,D,U,D,L,R</t>
+  </si>
+  <si>
+    <t>R,R,L,D,L,L</t>
+  </si>
+  <si>
+    <t>R,R,D,L,L,L</t>
+  </si>
+  <si>
+    <t>R,R,L,L,D,D,R</t>
+  </si>
+  <si>
+    <t>D,U,U,U,D,D,U,D</t>
+  </si>
+  <si>
+    <t>R,R,D,D,L,R</t>
+  </si>
+  <si>
+    <t>D,U,D,D,U,D</t>
+  </si>
+  <si>
+    <t>D,U,R,R,R,R,U,D</t>
+  </si>
+  <si>
+    <t>D,U,D,D,U,D,U,R</t>
+  </si>
+  <si>
+    <t>R,L,D,D,R,D</t>
+  </si>
+  <si>
+    <t>R,L,R,R,D,D,U,U</t>
+  </si>
+  <si>
+    <t>D,D,R,R,U,U,L</t>
+  </si>
+  <si>
+    <t>R,D,D,R,L,U</t>
+  </si>
+  <si>
+    <t>D,D,R,R,L</t>
+  </si>
+  <si>
+    <t>D,R,R,U,D,D,L,R</t>
+  </si>
+  <si>
+    <t>D,U,R,R,D,D,L,R</t>
+  </si>
+  <si>
+    <t>R,D,R,D,L,L,R,R</t>
+  </si>
+  <si>
+    <t>D,D,R,U,R,L,L,D</t>
+  </si>
+  <si>
+    <t>R,L,D,D,R,R</t>
+  </si>
+  <si>
+    <t>R,R,U,D,L,L,D,D</t>
+  </si>
+  <si>
+    <t>D,U,R,R,R</t>
+  </si>
+  <si>
+    <t>R,D,D,L,L,U,U</t>
+  </si>
+  <si>
+    <t>D,L,R,U,R,R,D</t>
+  </si>
+  <si>
+    <t>R,D,U,D,R,D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -510,8 +666,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,6 +899,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -900,7 +1066,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -928,6 +1094,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1284,18 +1453,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CB479"/>
+  <dimension ref="A1:CB481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="13" customWidth="1"/>
   </cols>
@@ -3201,13 +3370,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B18" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="C18" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D18" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="5"/>
@@ -3307,13 +3479,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B19" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="C19" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D19" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="5"/>
@@ -3410,13 +3585,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B20" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="C20" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D20" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="5"/>
@@ -3517,13 +3695,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B21" s="13" t="s">
+        <v>112</v>
+      </c>
       <c r="C21" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D21" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="5"/>
@@ -3611,11 +3792,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B22" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="C22" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D22" s="12" t="b">
+        <v>6</v>
+      </c>
+      <c r="D22" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3707,11 +3891,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B23" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="C23" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D23" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D23" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3806,11 +3993,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B24" s="13" t="s">
+        <v>114</v>
+      </c>
       <c r="C24" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D24" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3905,11 +4095,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B25" s="13" t="s">
+        <v>115</v>
+      </c>
       <c r="C25" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D25" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D25" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4002,11 +4195,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B26" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="C26" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D26" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D26" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4100,13 +4296,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B27" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="C27" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D27" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="5"/>
@@ -4201,11 +4400,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B28" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="C28" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D28" s="12" t="b">
+        <v>6</v>
+      </c>
+      <c r="D28" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4302,11 +4504,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B29" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="C29" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D29" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D29" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4403,13 +4608,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B30" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="C30" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D30" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="5"/>
@@ -4501,11 +4709,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B31" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="C31" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D31" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D31" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4607,11 +4818,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B32" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="C32" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="12" t="b">
+        <v>10</v>
+      </c>
+      <c r="D32" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4713,11 +4927,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B33" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="C33" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D33" s="12" t="b">
+        <v>6</v>
+      </c>
+      <c r="D33" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4819,11 +5036,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B34" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="C34" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D34" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D34" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4917,11 +5137,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B35" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="C35" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D35" s="12" t="b">
+        <v>9</v>
+      </c>
+      <c r="D35" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5018,13 +5241,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B36" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="C36" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D36" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="5"/>
@@ -5124,13 +5350,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B37" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="C37" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D37" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="5"/>
@@ -5230,13 +5459,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B38" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="C38" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D38" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="4">
         <f t="shared" si="5"/>
@@ -5336,13 +5568,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B39" s="13" t="s">
+        <v>128</v>
+      </c>
       <c r="C39" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D39" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="4">
         <f t="shared" si="5"/>
@@ -5443,13 +5678,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B40" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="C40" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D40" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="5"/>
@@ -5549,13 +5787,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B41" s="13" t="s">
+        <v>130</v>
+      </c>
       <c r="C41" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D41" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" si="5"/>
@@ -5656,13 +5897,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B42" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="C42" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D42" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" si="5"/>
@@ -5762,13 +6006,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B43" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="C43" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D43" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" si="5"/>
@@ -5868,13 +6115,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B44" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="C44" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D44" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="5"/>
@@ -5974,13 +6224,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B45" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="C45" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D45" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" si="5"/>
@@ -6080,13 +6333,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B46" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="C46" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D46" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="5"/>
@@ -6187,13 +6443,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B47" s="13" t="s">
+        <v>137</v>
+      </c>
       <c r="C47" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D47" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="5"/>
@@ -6293,11 +6552,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B48" s="13" t="s">
+        <v>138</v>
+      </c>
       <c r="C48" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="12" t="b">
+        <v>6</v>
+      </c>
+      <c r="D48" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6391,11 +6653,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B49" s="13" t="s">
+        <v>139</v>
+      </c>
       <c r="C49" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D49" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D49" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6497,11 +6762,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B50" s="13" t="s">
+        <v>140</v>
+      </c>
       <c r="C50" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D50" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D50" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6598,11 +6866,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B51" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="C51" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D51" s="12" t="b">
+        <v>6</v>
+      </c>
+      <c r="D51" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6704,11 +6975,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B52" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="C52" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D52" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D52" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6804,13 +7078,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B53" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="C53" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D53" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="4">
         <f t="shared" si="5"/>
@@ -6910,13 +7187,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B54" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="C54" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D54" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="4">
         <f t="shared" si="5"/>
@@ -7017,13 +7297,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B55" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C55" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D55" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="4">
         <f t="shared" si="5"/>
@@ -7123,13 +7406,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B56" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="C56" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D56" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4">
         <f t="shared" si="5"/>
@@ -7229,13 +7515,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B57" s="13" t="s">
+        <v>147</v>
+      </c>
       <c r="C57" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D57" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="4">
         <f t="shared" si="5"/>
@@ -7335,11 +7624,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B58" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="C58" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D58" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D58" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7436,11 +7728,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B59" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="C59" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D59" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D59" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7542,13 +7837,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B60" s="13" t="s">
+        <v>149</v>
+      </c>
       <c r="C60" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D60" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="4">
         <f t="shared" si="5"/>
@@ -7643,13 +7941,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B61" s="13" t="s">
+        <v>106</v>
+      </c>
       <c r="C61" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D61" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" s="4">
         <f t="shared" si="5"/>
@@ -7749,13 +8050,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B62" s="13" t="s">
+        <v>150</v>
+      </c>
       <c r="C62" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D62" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="4">
         <f t="shared" si="5"/>
@@ -7855,11 +8159,14 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B63" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="C63" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D63" s="12" t="b">
+        <v>8</v>
+      </c>
+      <c r="D63" s="14" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7956,13 +8263,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B64" s="13" t="s">
+        <v>151</v>
+      </c>
       <c r="C64" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D64" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="4">
         <f t="shared" si="5"/>
@@ -8062,13 +8372,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B65" s="13" t="s">
+        <v>152</v>
+      </c>
       <c r="C65" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D65" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="4">
         <f t="shared" si="5"/>
@@ -8168,13 +8481,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B66" s="13" t="s">
+        <v>153</v>
+      </c>
       <c r="C66" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D66" s="12" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" s="4">
         <f t="shared" si="5"/>
@@ -8274,13 +8590,16 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="B67" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="C67" s="12">
         <f t="shared" ref="C67:C130" si="7">LEN(B67)-LEN(SUBSTITUTE(B67,",",""))+1</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D67" s="12" t="b">
         <f t="shared" ref="D67:D130" si="8">C67=G67</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" s="4">
         <f t="shared" si="5"/>
@@ -8380,13 +8699,16 @@
         <f t="shared" ref="A68:A131" si="9">COUNTA(I68:N68)</f>
         <v>3</v>
       </c>
+      <c r="B68" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="C68" s="12">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D68" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="4">
         <f t="shared" ref="E68:E131" si="10">E67+1</f>
@@ -8487,13 +8809,16 @@
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
+      <c r="B69" s="13" t="s">
+        <v>155</v>
+      </c>
       <c r="C69" s="12">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D69" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="4">
         <f t="shared" si="10"/>
@@ -71774,7 +72099,7 @@
         <v>0</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E479" si="40">E451+1</f>
+        <f t="shared" ref="E452:E481" si="40">E451+1</f>
         <v>450</v>
       </c>
       <c r="F452" s="4">
@@ -77691,6 +78016,462 @@
         <v>78</v>
       </c>
       <c r="CB479" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="480" spans="1:80" x14ac:dyDescent="0.2">
+      <c r="A480" s="3">
+        <f t="shared" ref="A480:A481" si="42">COUNTA(I480:N480)</f>
+        <v>6</v>
+      </c>
+      <c r="C480" s="12">
+        <f t="shared" ref="C480:C481" si="43">LEN(B480)-LEN(SUBSTITUTE(B480,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="D480" s="12" t="b">
+        <f t="shared" ref="D480:D481" si="44">C480=G480</f>
+        <v>0</v>
+      </c>
+      <c r="E480" s="4">
+        <f t="shared" si="40"/>
+        <v>478</v>
+      </c>
+      <c r="F480" s="4">
+        <f t="shared" ref="F480:F481" si="45">E480</f>
+        <v>478</v>
+      </c>
+      <c r="G480" s="9">
+        <v>22</v>
+      </c>
+      <c r="H480" s="9">
+        <v>1</v>
+      </c>
+      <c r="I480" t="s">
+        <v>75</v>
+      </c>
+      <c r="J480" t="s">
+        <v>88</v>
+      </c>
+      <c r="K480" t="s">
+        <v>88</v>
+      </c>
+      <c r="L480" t="s">
+        <v>88</v>
+      </c>
+      <c r="M480" t="s">
+        <v>88</v>
+      </c>
+      <c r="N480" t="s">
+        <v>88</v>
+      </c>
+      <c r="O480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="R480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="S480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="U480" t="s">
+        <v>88</v>
+      </c>
+      <c r="V480" t="s">
+        <v>88</v>
+      </c>
+      <c r="W480" t="s">
+        <v>88</v>
+      </c>
+      <c r="X480" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y480" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL480" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ480" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR480" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT480" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU480" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV480" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW480" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX480" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY480" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ480" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA480" s="11"/>
+      <c r="BB480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC480" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE480" t="s">
+        <v>87</v>
+      </c>
+      <c r="BF480" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH480" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ480" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK480" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM480" s="11"/>
+      <c r="BN480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP480" s="11"/>
+      <c r="BQ480" t="s">
+        <v>78</v>
+      </c>
+      <c r="BR480" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS480" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT480" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU480" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV480" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW480" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ480" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA480" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="CB480" s="11"/>
+    </row>
+    <row r="481" spans="1:80" x14ac:dyDescent="0.2">
+      <c r="A481" s="3">
+        <f t="shared" si="42"/>
+        <v>6</v>
+      </c>
+      <c r="B481" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C481" s="12">
+        <f t="shared" si="43"/>
+        <v>30</v>
+      </c>
+      <c r="D481" s="12" t="b">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="E481" s="4">
+        <f t="shared" si="40"/>
+        <v>479</v>
+      </c>
+      <c r="F481" s="4">
+        <f t="shared" si="45"/>
+        <v>479</v>
+      </c>
+      <c r="G481" s="9">
+        <v>30</v>
+      </c>
+      <c r="H481" s="9">
+        <v>1</v>
+      </c>
+      <c r="I481" t="s">
+        <v>75</v>
+      </c>
+      <c r="J481" t="s">
+        <v>88</v>
+      </c>
+      <c r="K481" t="s">
+        <v>88</v>
+      </c>
+      <c r="L481" t="s">
+        <v>88</v>
+      </c>
+      <c r="M481" t="s">
+        <v>88</v>
+      </c>
+      <c r="N481" t="s">
+        <v>88</v>
+      </c>
+      <c r="O481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="R481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="S481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="U481" t="s">
+        <v>88</v>
+      </c>
+      <c r="V481" t="s">
+        <v>88</v>
+      </c>
+      <c r="W481" t="s">
+        <v>88</v>
+      </c>
+      <c r="X481" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y481" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL481" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ481" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR481" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT481" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU481" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV481" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW481" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX481" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ481" s="11"/>
+      <c r="BA481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB481" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC481" s="11"/>
+      <c r="BD481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE481" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF481" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG481" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH481" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI481" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL481" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN481" s="11"/>
+      <c r="BO481" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="BP481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BQ481" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR481" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS481" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT481" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU481" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV481" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX481" s="11"/>
+      <c r="BY481" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BZ481" s="11"/>
+      <c r="CA481" s="11"/>
+      <c r="CB481" s="11" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>